<commit_message>
Added hellinger distance as function
</commit_message>
<xml_diff>
--- a/experiments/models/LSTM_Sepsis_Case_u=32_e=inf_ep=5/training_metrics.xlsx
+++ b/experiments/models/LSTM_Sepsis_Case_u=32_e=inf_ep=5/training_metrics.xlsx
@@ -760,193 +760,193 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1570077687501907</v>
+        <v>0.129763126373291</v>
       </c>
       <c r="C2" t="n">
-        <v>5.724195957183838</v>
+        <v>5.631661415100098</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1527946889400482</v>
+        <v>0.1128171533346176</v>
       </c>
       <c r="E2" t="n">
-        <v>5.66736364364624</v>
+        <v>5.841971397399902</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1345379650592804</v>
+        <v>0.1327591091394424</v>
       </c>
       <c r="G2" t="n">
-        <v>5.757717609405518</v>
+        <v>5.727101802825928</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1201198399066925</v>
+        <v>0.1152513846755028</v>
       </c>
       <c r="I2" t="n">
-        <v>5.863194465637207</v>
+        <v>5.81063175201416</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1435258835554123</v>
+        <v>0.1567268967628479</v>
       </c>
       <c r="K2" t="n">
-        <v>5.766807079315186</v>
+        <v>5.790315628051758</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1109446659684181</v>
+        <v>0.1466154903173447</v>
       </c>
       <c r="M2" t="n">
-        <v>5.811973094940186</v>
+        <v>5.751532554626465</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1550416648387909</v>
+        <v>0.1308866143226624</v>
       </c>
       <c r="O2" t="n">
-        <v>5.732943058013916</v>
+        <v>5.737089157104492</v>
       </c>
       <c r="P2" t="n">
-        <v>0.1186218485236168</v>
+        <v>0.1271416544914246</v>
       </c>
       <c r="Q2" t="n">
-        <v>5.730655670166016</v>
+        <v>5.700167179107666</v>
       </c>
       <c r="R2" t="n">
-        <v>0.118247352540493</v>
+        <v>0.1223668232560158</v>
       </c>
       <c r="S2" t="n">
-        <v>5.762578964233398</v>
+        <v>5.729527950286865</v>
       </c>
       <c r="T2" t="n">
-        <v>0.1347252130508423</v>
+        <v>0.09736915677785873</v>
       </c>
       <c r="U2" t="n">
-        <v>5.791421890258789</v>
+        <v>5.677004814147949</v>
       </c>
       <c r="V2" t="n">
-        <v>0.1339762210845947</v>
+        <v>0.1045782193541527</v>
       </c>
       <c r="W2" t="n">
-        <v>5.779135227203369</v>
+        <v>5.70580530166626</v>
       </c>
       <c r="X2" t="n">
-        <v>0.1147832572460175</v>
+        <v>0.129763126373291</v>
       </c>
       <c r="Y2" t="n">
-        <v>5.826395034790039</v>
+        <v>5.803348541259766</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.1429641395807266</v>
+        <v>0.09596479684114456</v>
       </c>
       <c r="AA2" t="n">
-        <v>5.758456230163574</v>
+        <v>5.740166187286377</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.1362231969833374</v>
+        <v>0.1541990488767624</v>
       </c>
       <c r="AC2" t="n">
-        <v>5.782821178436279</v>
+        <v>5.806633472442627</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.1244265511631966</v>
+        <v>0.1325718611478806</v>
       </c>
       <c r="AE2" t="n">
-        <v>5.771160125732422</v>
+        <v>5.77132511138916</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.1404362916946411</v>
+        <v>0.1203070878982544</v>
       </c>
       <c r="AG2" t="n">
-        <v>5.689271926879883</v>
+        <v>5.686591148376465</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.1201198399066925</v>
+        <v>0.1432450115680695</v>
       </c>
       <c r="AI2" t="n">
-        <v>5.720421314239502</v>
+        <v>5.629205226898193</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.10233124345541</v>
+        <v>0.1145960092544556</v>
       </c>
       <c r="AK2" t="n">
-        <v>5.732498645782471</v>
+        <v>5.692140102386475</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.1309802383184433</v>
+        <v>0.1154386326670647</v>
       </c>
       <c r="AM2" t="n">
-        <v>5.710404872894287</v>
+        <v>5.687292575836182</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.126392662525177</v>
+        <v>0.1259245425462723</v>
       </c>
       <c r="AO2" t="n">
-        <v>5.723645687103271</v>
+        <v>5.715898990631104</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.1568205207586288</v>
+        <v>0.1048590987920761</v>
       </c>
       <c r="AQ2" t="n">
-        <v>5.78359317779541</v>
+        <v>5.761429786682129</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.1429641395807266</v>
+        <v>0.1322909891605377</v>
       </c>
       <c r="AS2" t="n">
-        <v>5.689394474029541</v>
+        <v>5.80755090713501</v>
       </c>
       <c r="AT2" t="n">
-        <v>0.0730268731713295</v>
+        <v>0.131822869181633</v>
       </c>
       <c r="AU2" t="n">
-        <v>5.733864307403564</v>
+        <v>5.679728507995605</v>
       </c>
       <c r="AV2" t="n">
-        <v>0.1228349432349205</v>
+        <v>0.1459601223468781</v>
       </c>
       <c r="AW2" t="n">
-        <v>5.796497344970703</v>
+        <v>5.61656665802002</v>
       </c>
       <c r="AX2" t="n">
-        <v>0.1444621235132217</v>
+        <v>0.08959835022687912</v>
       </c>
       <c r="AY2" t="n">
-        <v>5.843997955322266</v>
+        <v>5.879850387573242</v>
       </c>
       <c r="AZ2" t="n">
-        <v>0.1300439983606339</v>
+        <v>0.1379084289073944</v>
       </c>
       <c r="BA2" t="n">
-        <v>5.73823070526123</v>
+        <v>5.695398807525635</v>
       </c>
       <c r="BB2" t="n">
-        <v>0.08004868775606155</v>
+        <v>0.07321412116289139</v>
       </c>
       <c r="BC2" t="n">
-        <v>5.68825101852417</v>
+        <v>5.815468311309814</v>
       </c>
       <c r="BD2" t="n">
-        <v>0.1195580959320068</v>
+        <v>0.1248946711421013</v>
       </c>
       <c r="BE2" t="n">
-        <v>5.801265239715576</v>
+        <v>5.751345634460449</v>
       </c>
       <c r="BF2" t="n">
-        <v>0.1184346005320549</v>
+        <v>0.1407171636819839</v>
       </c>
       <c r="BG2" t="n">
-        <v>5.735671043395996</v>
+        <v>5.755179882049561</v>
       </c>
       <c r="BH2" t="n">
-        <v>0.1073869466781616</v>
+        <v>0.1163748726248741</v>
       </c>
       <c r="BI2" t="n">
-        <v>5.783974647521973</v>
+        <v>5.749183654785156</v>
       </c>
       <c r="BJ2" t="n">
-        <v>0.1468027383089066</v>
+        <v>0.1384701877832413</v>
       </c>
       <c r="BK2" t="n">
-        <v>5.835712909698486</v>
+        <v>5.751509189605713</v>
       </c>
       <c r="BL2" t="n">
-        <v>178.5345458984375</v>
+        <v>177.8996887207031</v>
       </c>
     </row>
     <row r="3">
@@ -954,193 +954,193 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2023218870162964</v>
+        <v>0.161969855427742</v>
       </c>
       <c r="C3" t="n">
-        <v>3.883747577667236</v>
+        <v>3.86277174949646</v>
       </c>
       <c r="D3" t="n">
-        <v>0.177885964512825</v>
+        <v>0.2043816149234772</v>
       </c>
       <c r="E3" t="n">
-        <v>3.945072174072266</v>
+        <v>4.040936946868896</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1715195178985596</v>
+        <v>0.1662765592336655</v>
       </c>
       <c r="G3" t="n">
-        <v>3.975829124450684</v>
+        <v>3.97049880027771</v>
       </c>
       <c r="H3" t="n">
+        <v>0.2239490747451782</v>
+      </c>
+      <c r="I3" t="n">
+        <v>4.10195255279541</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.1830352991819382</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3.980755567550659</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.1755453646183014</v>
+      </c>
+      <c r="M3" t="n">
+        <v>3.943369388580322</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.1832225471735001</v>
+      </c>
+      <c r="O3" t="n">
+        <v>3.959116697311401</v>
+      </c>
+      <c r="P3" t="n">
         <v>0.2017601281404495</v>
       </c>
-      <c r="I3" t="n">
-        <v>4.122687339782715</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.1718003898859024</v>
-      </c>
-      <c r="K3" t="n">
-        <v>3.982381343841553</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.176294356584549</v>
-      </c>
-      <c r="M3" t="n">
-        <v>3.965460300445557</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.2055987268686295</v>
-      </c>
-      <c r="O3" t="n">
-        <v>3.945102691650391</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.1909933537244797</v>
-      </c>
       <c r="Q3" t="n">
-        <v>3.920292139053345</v>
+        <v>3.89659309387207</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1626252233982086</v>
+        <v>0.2434228956699371</v>
       </c>
       <c r="S3" t="n">
-        <v>3.969719409942627</v>
+        <v>3.950108289718628</v>
       </c>
       <c r="T3" t="n">
-        <v>0.2051306068897247</v>
+        <v>0.1931467056274414</v>
       </c>
       <c r="U3" t="n">
-        <v>3.992314338684082</v>
+        <v>3.891482353210449</v>
       </c>
       <c r="V3" t="n">
-        <v>0.1944574415683746</v>
+        <v>0.1589738726615906</v>
       </c>
       <c r="W3" t="n">
-        <v>3.960981845855713</v>
+        <v>3.947196245193481</v>
       </c>
       <c r="X3" t="n">
-        <v>0.2024155110120773</v>
+        <v>0.193895697593689</v>
       </c>
       <c r="Y3" t="n">
-        <v>4.138921737670898</v>
+        <v>4.126945972442627</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.1826608031988144</v>
+        <v>0.2089691907167435</v>
       </c>
       <c r="AA3" t="n">
-        <v>3.961338758468628</v>
+        <v>3.939017772674561</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.1970789283514023</v>
+        <v>0.226008802652359</v>
       </c>
       <c r="AC3" t="n">
-        <v>3.952458381652832</v>
+        <v>3.967980146408081</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.1903379857540131</v>
+        <v>0.2090628147125244</v>
       </c>
       <c r="AE3" t="n">
-        <v>3.94395899772644</v>
+        <v>3.908987045288086</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.1848141551017761</v>
+        <v>0.2113098055124283</v>
       </c>
       <c r="AG3" t="n">
-        <v>3.873656272888184</v>
+        <v>3.862776279449463</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.1767624765634537</v>
+        <v>0.21346315741539</v>
       </c>
       <c r="AI3" t="n">
-        <v>3.930212259292603</v>
+        <v>3.88976526260376</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.1830352991819382</v>
+        <v>0.1931467056274414</v>
       </c>
       <c r="AK3" t="n">
-        <v>3.96045994758606</v>
+        <v>3.933079242706299</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.2144930213689804</v>
+        <v>0.1971725523471832</v>
       </c>
       <c r="AM3" t="n">
-        <v>3.916740655899048</v>
+        <v>3.91792368888855</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.1737665086984634</v>
+        <v>0.174515500664711</v>
       </c>
       <c r="AO3" t="n">
-        <v>3.956692218780518</v>
+        <v>3.949765920639038</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.200917512178421</v>
+        <v>0.215242013335228</v>
       </c>
       <c r="AQ3" t="n">
-        <v>3.969424724578857</v>
+        <v>3.920153617858887</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.1923040896654129</v>
+        <v>0.2145866453647614</v>
       </c>
       <c r="AS3" t="n">
-        <v>3.890201568603516</v>
+        <v>3.960657358169556</v>
       </c>
       <c r="AT3" t="n">
         <v>0.1670255661010742</v>
       </c>
       <c r="AU3" t="n">
-        <v>3.949291229248047</v>
+        <v>3.916486024856567</v>
       </c>
       <c r="AV3" t="n">
-        <v>0.1710513979196548</v>
+        <v>0.2141185253858566</v>
       </c>
       <c r="AW3" t="n">
-        <v>3.945626735687256</v>
+        <v>3.860432386398315</v>
       </c>
       <c r="AX3" t="n">
-        <v>0.2209530919790268</v>
+        <v>0.2155228853225708</v>
       </c>
       <c r="AY3" t="n">
-        <v>4.239065170288086</v>
+        <v>4.268998622894287</v>
       </c>
       <c r="AZ3" t="n">
-        <v>0.1978279203176498</v>
+        <v>0.2073775827884674</v>
       </c>
       <c r="BA3" t="n">
-        <v>3.916168212890625</v>
+        <v>3.884915828704834</v>
       </c>
       <c r="BB3" t="n">
-        <v>0.1865930110216141</v>
+        <v>0.1986705362796783</v>
       </c>
       <c r="BC3" t="n">
-        <v>3.918695449829102</v>
+        <v>4.026835441589355</v>
       </c>
       <c r="BD3" t="n">
-        <v>0.1592547446489334</v>
+        <v>0.2049433588981628</v>
       </c>
       <c r="BE3" t="n">
-        <v>4.022674560546875</v>
+        <v>3.937058925628662</v>
       </c>
       <c r="BF3" t="n">
-        <v>0.2089691907167435</v>
+        <v>0.1856567710638046</v>
       </c>
       <c r="BG3" t="n">
-        <v>3.985174417495728</v>
+        <v>3.999357461929321</v>
       </c>
       <c r="BH3" t="n">
-        <v>0.1592547446489334</v>
+        <v>0.1617826074361801</v>
       </c>
       <c r="BI3" t="n">
-        <v>4.068567276000977</v>
+        <v>4.057180404663086</v>
       </c>
       <c r="BJ3" t="n">
-        <v>0.2040071189403534</v>
+        <v>0.1774178445339203</v>
       </c>
       <c r="BK3" t="n">
-        <v>3.974307060241699</v>
+        <v>3.942774772644043</v>
       </c>
       <c r="BL3" t="n">
-        <v>123.1788330078125</v>
+        <v>122.8174896240234</v>
       </c>
     </row>
     <row r="4">
@@ -1148,193 +1148,193 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2539088129997253</v>
+        <v>0.2622413635253906</v>
       </c>
       <c r="C4" t="n">
-        <v>2.584082841873169</v>
+        <v>2.597655057907104</v>
       </c>
       <c r="D4" t="n">
+        <v>0.2622413635253906</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.733408689498901</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.2701994180679321</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.677418231964111</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.2995038032531738</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2.85958194732666</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.2577474117279053</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2.660968065261841</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.2601816356182098</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2.631896495819092</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.2649564743041992</v>
+      </c>
+      <c r="O4" t="n">
+        <v>2.658324003219604</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.2528789341449738</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2.614120721817017</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.3287145495414734</v>
+      </c>
+      <c r="S4" t="n">
+        <v>2.647596597671509</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.265330970287323</v>
+      </c>
+      <c r="U4" t="n">
+        <v>2.627753019332886</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.2516618371009827</v>
+      </c>
+      <c r="W4" t="n">
+        <v>2.647079229354858</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.2689822912216187</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>2.907799959182739</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.2728208899497986</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>2.634251832962036</v>
+      </c>
+      <c r="AB4" t="n">
         <v>0.2660799622535706</v>
       </c>
-      <c r="E4" t="n">
-        <v>2.719221353530884</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.2572792768478394</v>
-      </c>
-      <c r="G4" t="n">
-        <v>2.6566002368927</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.2450145184993744</v>
-      </c>
-      <c r="I4" t="n">
-        <v>2.865227699279785</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.2333114892244339</v>
-      </c>
-      <c r="K4" t="n">
-        <v>2.669071912765503</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.274225264787674</v>
-      </c>
-      <c r="M4" t="n">
-        <v>2.616764783859253</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.2686077952384949</v>
-      </c>
-      <c r="O4" t="n">
-        <v>2.659040212631226</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0.265050083398819</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>2.616011619567871</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.2465125024318695</v>
-      </c>
-      <c r="S4" t="n">
-        <v>2.666894912719727</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0.2608369886875153</v>
-      </c>
-      <c r="U4" t="n">
-        <v>2.667007923126221</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0.2815279364585876</v>
-      </c>
-      <c r="W4" t="n">
-        <v>2.636168956756592</v>
-      </c>
-      <c r="X4" t="n">
-        <v>0.2813406884670258</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>2.897842407226562</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>0.2555004358291626</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>2.650901079177856</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>0.2467933744192123</v>
-      </c>
       <c r="AC4" t="n">
-        <v>2.626664161682129</v>
+        <v>2.616246223449707</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.254189670085907</v>
+        <v>0.2618668675422668</v>
       </c>
       <c r="AE4" t="n">
-        <v>2.608554363250732</v>
+        <v>2.590165853500366</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.2553131580352783</v>
+        <v>0.2732890248298645</v>
       </c>
       <c r="AG4" t="n">
-        <v>2.583624839782715</v>
+        <v>2.565396070480347</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.2337796092033386</v>
+        <v>0.279561847448349</v>
       </c>
       <c r="AI4" t="n">
-        <v>2.646368503570557</v>
+        <v>2.648171186447144</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.2558749318122864</v>
+        <v>0.2854601740837097</v>
       </c>
       <c r="AK4" t="n">
-        <v>2.680959224700928</v>
+        <v>2.645664691925049</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.2781574726104736</v>
+        <v>0.2908903658390045</v>
       </c>
       <c r="AM4" t="n">
-        <v>2.623953819274902</v>
+        <v>2.646908521652222</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.2580282688140869</v>
+        <v>0.2745061218738556</v>
       </c>
       <c r="AO4" t="n">
-        <v>2.667562246322632</v>
+        <v>2.662474155426025</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.2690759301185608</v>
+        <v>0.2851792871952057</v>
       </c>
       <c r="AQ4" t="n">
-        <v>2.637842178344727</v>
+        <v>2.58244800567627</v>
       </c>
       <c r="AR4" t="n">
-        <v>0.2483849823474884</v>
+        <v>0.2651437222957611</v>
       </c>
       <c r="AS4" t="n">
-        <v>2.591758728027344</v>
+        <v>2.620267152786255</v>
       </c>
       <c r="AT4" t="n">
-        <v>0.2421121597290039</v>
+        <v>0.2748806178569794</v>
       </c>
       <c r="AU4" t="n">
-        <v>2.657115459442139</v>
+        <v>2.631274223327637</v>
       </c>
       <c r="AV4" t="n">
-        <v>0.2487594783306122</v>
+        <v>0.2741316258907318</v>
       </c>
       <c r="AW4" t="n">
-        <v>2.612989664077759</v>
+        <v>2.584620237350464</v>
       </c>
       <c r="AX4" t="n">
-        <v>0.2755360007286072</v>
+        <v>0.2874262630939484</v>
       </c>
       <c r="AY4" t="n">
-        <v>3.102588653564453</v>
+        <v>3.118444442749023</v>
       </c>
       <c r="AZ4" t="n">
-        <v>0.2577474117279053</v>
+        <v>0.3002527952194214</v>
       </c>
       <c r="BA4" t="n">
-        <v>2.604429960250854</v>
+        <v>2.57660436630249</v>
       </c>
       <c r="BB4" t="n">
-        <v>0.2731017768383026</v>
+        <v>0.2484786063432693</v>
       </c>
       <c r="BC4" t="n">
-        <v>2.652142763137817</v>
+        <v>2.69646954536438</v>
       </c>
       <c r="BD4" t="n">
-        <v>0.268701434135437</v>
+        <v>0.2913585007190704</v>
       </c>
       <c r="BE4" t="n">
-        <v>2.699179887771606</v>
+        <v>2.634551048278809</v>
       </c>
       <c r="BF4" t="n">
-        <v>0.2689822912216187</v>
+        <v>0.2591517567634583</v>
       </c>
       <c r="BG4" t="n">
-        <v>2.750611066818237</v>
+        <v>2.758622407913208</v>
       </c>
       <c r="BH4" t="n">
-        <v>0.2495084702968597</v>
+        <v>0.2480104863643646</v>
       </c>
       <c r="BI4" t="n">
-        <v>2.872097015380859</v>
+        <v>2.855077266693115</v>
       </c>
       <c r="BJ4" t="n">
-        <v>0.2694504261016846</v>
+        <v>0.2533470690250397</v>
       </c>
       <c r="BK4" t="n">
-        <v>2.679919481277466</v>
+        <v>2.704269886016846</v>
       </c>
       <c r="BL4" t="n">
-        <v>83.20549011230469</v>
+        <v>83.03787994384766</v>
       </c>
     </row>
     <row r="5">
@@ -1342,193 +1342,193 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3522142171859741</v>
+        <v>0.3497799932956696</v>
       </c>
       <c r="C5" t="n">
-        <v>1.998591065406799</v>
+        <v>2.015238285064697</v>
       </c>
       <c r="D5" t="n">
+        <v>0.3832038342952728</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2.122657299041748</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.393127977848053</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2.063883066177368</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.378897100687027</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2.264148712158203</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.3845145702362061</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2.059808015823364</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.3604531288146973</v>
+      </c>
+      <c r="M5" t="n">
+        <v>2.03269100189209</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.3611085116863251</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2.058640956878662</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.3619511425495148</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>2.024381637573242</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.4074524939060211</v>
+      </c>
+      <c r="S5" t="n">
+        <v>2.046107292175293</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.3775863647460938</v>
+      </c>
+      <c r="U5" t="n">
+        <v>2.05682897567749</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.3958430886268616</v>
+      </c>
+      <c r="W5" t="n">
+        <v>2.051582813262939</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.3678494393825531</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>2.265000581741333</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.3882595300674438</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>2.052570819854736</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0.3881658911705017</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>2.006833553314209</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0.3789907395839691</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>1.998265266418457</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0.3786162436008453</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>1.99779486656189</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0.3958430886268616</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>2.057927131652832</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0.391442745923996</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>2.052738428115845</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0.400617927312851</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>2.054333925247192</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>0.3743095099925995</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>2.064586877822876</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0.3989326953887939</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>1.998428821563721</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>0.3656961023807526</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>2.011928558349609</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0.3961239457130432</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>2.053141355514526</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>0.3812377154827118</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>1.99893319606781</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>0.3717816770076752</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>2.418110132217407</v>
+      </c>
+      <c r="AZ5" t="n">
         <v>0.3731860220432281</v>
       </c>
-      <c r="E5" t="n">
-        <v>2.126782178878784</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.3664450943470001</v>
-      </c>
-      <c r="G5" t="n">
-        <v>2.061078310012817</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.3617638945579529</v>
-      </c>
-      <c r="I5" t="n">
-        <v>2.268641471862793</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.346596747636795</v>
-      </c>
-      <c r="K5" t="n">
-        <v>2.076081275939941</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.3674749433994293</v>
-      </c>
-      <c r="M5" t="n">
-        <v>2.029921770095825</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.3732796609401703</v>
-      </c>
-      <c r="O5" t="n">
-        <v>2.0682373046875</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.3600786328315735</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>2.024169921875</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.3776800036430359</v>
-      </c>
-      <c r="S5" t="n">
-        <v>2.061927318572998</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0.3701900541782379</v>
-      </c>
-      <c r="U5" t="n">
-        <v>2.065086364746094</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0.3657897114753723</v>
-      </c>
-      <c r="W5" t="n">
-        <v>2.051780462265015</v>
-      </c>
-      <c r="X5" t="n">
-        <v>0.364947110414505</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>2.27085018157959</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>0.3651343584060669</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>2.063288688659668</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>0.3514652252197266</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>2.03335165977478</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>0.3640108704566956</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>2.008469343185425</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>0.3514652252197266</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>2.00991678237915</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>0.3564273118972778</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>2.058725357055664</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>0.3552101850509644</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>2.078098058700562</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>0.3729987740516663</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>2.052136182785034</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>0.3657897114753723</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>2.080451250076294</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>0.3664450943470001</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>2.022561550140381</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>0.3513715863227844</v>
-      </c>
-      <c r="AS5" t="n">
-        <v>2.010773420333862</v>
-      </c>
-      <c r="AT5" t="n">
-        <v>0.3607340157032013</v>
-      </c>
-      <c r="AU5" t="n">
-        <v>2.070253849029541</v>
-      </c>
-      <c r="AV5" t="n">
-        <v>0.3528695702552795</v>
-      </c>
-      <c r="AW5" t="n">
-        <v>2.013948917388916</v>
-      </c>
-      <c r="AX5" t="n">
-        <v>0.3628873825073242</v>
-      </c>
-      <c r="AY5" t="n">
-        <v>2.416337728500366</v>
-      </c>
-      <c r="AZ5" t="n">
-        <v>0.3602658808231354</v>
-      </c>
       <c r="BA5" t="n">
-        <v>2.019659757614136</v>
+        <v>2.001971006393433</v>
       </c>
       <c r="BB5" t="n">
-        <v>0.3656024634838104</v>
+        <v>0.3372343480587006</v>
       </c>
       <c r="BC5" t="n">
-        <v>2.071651458740234</v>
+        <v>2.084642171859741</v>
       </c>
       <c r="BD5" t="n">
-        <v>0.3796460926532745</v>
+        <v>0.4082014858722687</v>
       </c>
       <c r="BE5" t="n">
-        <v>2.074694871902466</v>
+        <v>2.043863534927368</v>
       </c>
       <c r="BF5" t="n">
-        <v>0.3582997918128967</v>
+        <v>0.3795524835586548</v>
       </c>
       <c r="BG5" t="n">
-        <v>2.201759576797485</v>
+        <v>2.200766563415527</v>
       </c>
       <c r="BH5" t="n">
-        <v>0.3409793078899384</v>
+        <v>0.3677558302879333</v>
       </c>
       <c r="BI5" t="n">
-        <v>2.322292327880859</v>
+        <v>2.306447982788086</v>
       </c>
       <c r="BJ5" t="n">
-        <v>0.3566145598888397</v>
+        <v>0.3594232797622681</v>
       </c>
       <c r="BK5" t="n">
-        <v>2.126572608947754</v>
+        <v>2.138532400131226</v>
       </c>
       <c r="BL5" t="n">
-        <v>64.84133148193359</v>
+        <v>64.60597229003906</v>
       </c>
     </row>
     <row r="6">
@@ -1536,193 +1536,193 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4298286736011505</v>
+        <v>0.432450145483017</v>
       </c>
       <c r="C6" t="n">
-        <v>1.754390120506287</v>
+        <v>1.737592935562134</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4336672723293304</v>
+        <v>0.4480853974819183</v>
       </c>
       <c r="E6" t="n">
-        <v>1.876512408256531</v>
+        <v>1.848947763442993</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4362887442111969</v>
+        <v>0.4506132304668427</v>
       </c>
       <c r="G6" t="n">
-        <v>1.808178067207336</v>
+        <v>1.777076959609985</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4130699336528778</v>
+        <v>0.4424679279327393</v>
       </c>
       <c r="I6" t="n">
-        <v>2.02457070350647</v>
+        <v>2.002893924713135</v>
       </c>
       <c r="J6" t="n">
-        <v>0.4242112040519714</v>
+        <v>0.4502387344837189</v>
       </c>
       <c r="K6" t="n">
-        <v>1.825388193130493</v>
+        <v>1.777514934539795</v>
       </c>
       <c r="L6" t="n">
-        <v>0.4238367080688477</v>
+        <v>0.4303904175758362</v>
       </c>
       <c r="M6" t="n">
-        <v>1.782814025878906</v>
+        <v>1.760067939758301</v>
       </c>
       <c r="N6" t="n">
-        <v>0.4147551655769348</v>
+        <v>0.4417189359664917</v>
       </c>
       <c r="O6" t="n">
-        <v>1.817095756530762</v>
+        <v>1.78512704372406</v>
       </c>
       <c r="P6" t="n">
-        <v>0.4155977964401245</v>
+        <v>0.4395655691623688</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.777820110321045</v>
+        <v>1.744319438934326</v>
       </c>
       <c r="R6" t="n">
-        <v>0.4448085427284241</v>
+        <v>0.4574477970600128</v>
       </c>
       <c r="S6" t="n">
-        <v>1.806911587715149</v>
+        <v>1.774794101715088</v>
       </c>
       <c r="T6" t="n">
+        <v>0.4505196213722229</v>
+      </c>
+      <c r="U6" t="n">
+        <v>1.77809751033783</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.4558562040328979</v>
+      </c>
+      <c r="W6" t="n">
+        <v>1.775747537612915</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.3979964554309845</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>1.948885083198547</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.4424679279327393</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>1.777356743812561</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.4364759922027588</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>1.740732669830322</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.4462128877639771</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>1.726623892784119</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0.4461192786693573</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>1.732983946800232</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0.4505196213722229</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>1.772844433784485</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0.4569796919822693</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>1.775307059288025</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.4483662545681</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>1.772117972373962</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0.4413444399833679</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>1.790403962135315</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0.459226667881012</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>1.731085896492004</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>0.4494897425174713</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>1.72825562953949</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.442842423915863</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>1.779782176017761</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.4452766478061676</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>1.723855495452881</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.3938769698143005</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>2.063251972198486</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>0.4352588653564453</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>1.736462116241455</v>
+      </c>
+      <c r="BB6" t="n">
         <v>0.4354461133480072</v>
       </c>
-      <c r="U6" t="n">
-        <v>1.815688371658325</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0.443310558795929</v>
-      </c>
-      <c r="W6" t="n">
-        <v>1.802549123764038</v>
-      </c>
-      <c r="X6" t="n">
-        <v>0.3841400742530823</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>1.979487538337708</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>0.4390038251876831</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>1.813679218292236</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>0.4064226150512695</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>1.781424760818481</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>0.419904500246048</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>1.759765863418579</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>0.4318884015083313</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>1.762617111206055</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>0.4403145909309387</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>1.797780156135559</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>0.4387229681015015</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>1.821144342422485</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>0.4402209520339966</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>1.807574868202209</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>0.4099803268909454</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>1.825897574424744</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>0.4175638854503632</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>1.772373199462891</v>
-      </c>
-      <c r="AR6" t="n">
-        <v>0.4170957803726196</v>
-      </c>
-      <c r="AS6" t="n">
-        <v>1.761557459831238</v>
-      </c>
-      <c r="AT6" t="n">
-        <v>0.4363823533058167</v>
-      </c>
-      <c r="AU6" t="n">
-        <v>1.812731266021729</v>
-      </c>
-      <c r="AV6" t="n">
-        <v>0.4288924336433411</v>
-      </c>
-      <c r="AW6" t="n">
-        <v>1.760503053665161</v>
-      </c>
-      <c r="AX6" t="n">
-        <v>0.3902256488800049</v>
-      </c>
-      <c r="AY6" t="n">
-        <v>2.083833694458008</v>
-      </c>
-      <c r="AZ6" t="n">
-        <v>0.4305776655673981</v>
-      </c>
-      <c r="BA6" t="n">
-        <v>1.761846780776978</v>
-      </c>
-      <c r="BB6" t="n">
-        <v>0.4098867177963257</v>
-      </c>
       <c r="BC6" t="n">
-        <v>1.821532487869263</v>
+        <v>1.801616787910461</v>
       </c>
       <c r="BD6" t="n">
-        <v>0.4409699440002441</v>
+        <v>0.4569796919822693</v>
       </c>
       <c r="BE6" t="n">
-        <v>1.817484259605408</v>
+        <v>1.769651889801025</v>
       </c>
       <c r="BF6" t="n">
-        <v>0.4294541776180267</v>
+        <v>0.4381612241268158</v>
       </c>
       <c r="BG6" t="n">
-        <v>1.968244194984436</v>
+        <v>1.942425727844238</v>
       </c>
       <c r="BH6" t="n">
-        <v>0.4094185829162598</v>
+        <v>0.4512686133384705</v>
       </c>
       <c r="BI6" t="n">
-        <v>2.091048002243042</v>
+        <v>2.050607442855835</v>
       </c>
       <c r="BJ6" t="n">
-        <v>0.4084823429584503</v>
+        <v>0.4226196110248566</v>
       </c>
       <c r="BK6" t="n">
-        <v>1.896180629730225</v>
+        <v>1.872190594673157</v>
       </c>
       <c r="BL6" t="n">
-        <v>56.99303817749023</v>
+        <v>56.00297927856445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>